<commit_message>
Author : Ruchit Jain Description : Updated Excel sheets as per modifications done as per user requirements               updated master sql for create tables-withPC.sql( set job role code,level to nullable & tpId,centerId to not null in Batch table
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/SCGJ_Updated_Excel/Batch.xlsx
+++ b/SSDMS_Requirements/SCGJ_Updated_Excel/Batch.xlsx
@@ -78,9 +78,6 @@
     <t>Integer</t>
   </si>
   <si>
-    <t>Market Mode/Surya Mitra/NDC/FDC</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>PMKVY/NON-PMKVY</t>
+  </si>
+  <si>
+    <t>Market Mode/Surya Mitra/NBCFDC</t>
   </si>
 </sst>
 </file>
@@ -226,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -283,6 +283,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,7 +594,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -624,7 +630,7 @@
   <sheetData>
     <row r="1" spans="1:25" s="19" customFormat="1">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -633,13 +639,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="20" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>2</v>
@@ -656,7 +662,7 @@
       <c r="K1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="21" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="12" t="s">
@@ -665,7 +671,7 @@
       <c r="N1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="21" t="s">
         <v>10</v>
       </c>
       <c r="P1" s="12" t="s">
@@ -693,10 +699,10 @@
         <v>18</v>
       </c>
       <c r="X1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" s="15" t="s">
         <v>26</v>
-      </c>
-      <c r="Y1" s="15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="19" customFormat="1">
@@ -704,53 +710,53 @@
         <v>19</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="16" t="s">
+      <c r="L2" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>21</v>
-      </c>
       <c r="R2" s="16" t="s">
         <v>19</v>
       </c>
@@ -764,10 +770,10 @@
         <v>19</v>
       </c>
       <c r="V2" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W2" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="X2" s="16" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Author : Ruchit Jain Description : Updated Batch and Candidate Excel sheet. UpdateCandidateAndBatchTable.sql file added to make DB fir for changes made
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/SCGJ_Updated_Excel/Batch.xlsx
+++ b/SSDMS_Requirements/SCGJ_Updated_Excel/Batch.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
   <si>
     <t>batchName</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>PMKVY/NON-PMKVY</t>
-  </si>
-  <si>
-    <t>Market Mode/Surya Mitra/NBCFDC</t>
   </si>
 </sst>
 </file>
@@ -594,7 +591,7 @@
   <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -728,7 +725,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Author: Ruchit Jain Description : Updated Batch excel sheet to give a drop down list in BatchMode column.
</commit_message>
<xml_diff>
--- a/SSDMS_Requirements/SCGJ_Updated_Excel/Batch.xlsx
+++ b/SSDMS_Requirements/SCGJ_Updated_Excel/Batch.xlsx
@@ -11,12 +11,16 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="Any">[0]!BatchMode</definedName>
+    <definedName name="BatchMode">Sheet2!$A$2:$A$10</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>batchName</t>
   </si>
@@ -112,6 +116,39 @@
   </si>
   <si>
     <t>PMKVY/NON-PMKVY</t>
+  </si>
+  <si>
+    <t>BatchMode</t>
+  </si>
+  <si>
+    <t>PMKVY-RPL</t>
+  </si>
+  <si>
+    <t>PMKVY-STT</t>
+  </si>
+  <si>
+    <t>PMKVY-Special</t>
+  </si>
+  <si>
+    <t>NSKFDC</t>
+  </si>
+  <si>
+    <t>NBCFDC</t>
+  </si>
+  <si>
+    <t>CB_Scheme</t>
+  </si>
+  <si>
+    <t>State Skill</t>
+  </si>
+  <si>
+    <t>MNRE</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>Select from DropDown List</t>
   </si>
 </sst>
 </file>
@@ -223,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -285,6 +322,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -725,7 +765,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="I2" s="18" t="s">
         <v>20</v>
@@ -781,6 +821,11 @@
     </row>
   </sheetData>
   <sheetProtection password="C97D" sheet="1" objects="1" scenarios="1" deleteRows="0"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H1048576">
+      <formula1>BatchMode</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -788,13 +833,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>